<commit_message>
Fixed OreSat0.1 BOM - debug connector was wrong. Also added PCB cost.
</commit_message>
<xml_diff>
--- a/oresat0-backplane-bom.xlsx
+++ b/oresat0-backplane-bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19" count="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17" count="17">
   <si>
     <t>Notes</t>
   </si>
@@ -54,6 +54,9 @@
     <t>N</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>Rohm</t>
   </si>
   <si>
@@ -67,15 +70,6 @@
   </si>
   <si>
     <t>High wattage just in case</t>
-  </si>
-  <si>
-    <t>BOM Version Information</t>
-  </si>
-  <si>
-    <t>Rev</t>
-  </si>
-  <si>
-    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -149,24 +143,24 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
       <protection locked="1" hidden="0"/>
     </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="100" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="100" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
       <protection locked="1" hidden="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
       <protection locked="1" hidden="0"/>
     </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="100" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="100" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
       <protection locked="1" hidden="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0">
@@ -201,7 +195,7 @@
   <dimension ref="A1:U1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -214,10 +208,9 @@
     <col min="6" max="6" style="0" width="57.567968750000006" customWidth="1"/>
     <col min="7" max="7" style="0" width="11.427884615384617" customWidth="1"/>
     <col min="8" max="8" style="0" width="27.712620192307696" customWidth="1"/>
-    <col min="9" max="9" style="1" width="9.142307692307693"/>
-    <col min="10" max="10" style="2" width="9.142307692307693"/>
-    <col min="11" max="11" style="2" width="10.856490384615386" customWidth="1"/>
-    <col min="12" max="12" style="1" width="9.142307692307693"/>
+    <col min="9" max="9" style="1" width="9.285156250000002" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" style="1" width="10.856490384615386" customWidth="1"/>
+    <col min="11" max="12" style="2" width="9.142307692307693"/>
     <col min="13" max="13" style="0" width="42.71171875" customWidth="1"/>
     <col min="14" max="17" style="0" width="9.142307692307693"/>
     <col min="18" max="18" style="0" width="27.855468750000004" customWidth="1"/>
@@ -241,9 +234,9 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="5"/>
+      <c r="J1" s="4"/>
       <c r="K1" s="5"/>
-      <c r="L1" s="4"/>
+      <c r="L1" s="5"/>
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:21" ht="13.5">
@@ -268,15 +261,15 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="5"/>
+      <c r="J2" s="4"/>
       <c r="K2" s="5"/>
-      <c r="L2" s="4"/>
+      <c r="L2" s="5"/>
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:21" ht="13.5">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>BOM revision: 0</t>
+          <t>BOM revision: 1</t>
         </is>
       </c>
       <c r="B3" s="3"/>
@@ -295,9 +288,9 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="5"/>
+      <c r="J3" s="4"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="4"/>
+      <c r="L3" s="5"/>
       <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:21">
@@ -310,9 +303,9 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="5"/>
+      <c r="J4" s="4"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="4"/>
+      <c r="L4" s="5"/>
       <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:21" ht="13.5">
@@ -356,19 +349,19 @@
           <t>Dist. PN</t>
         </is>
       </c>
-      <c r="I5" s="7" t="inlineStr">
-        <is>
-          <t>Stock</t>
+      <c r="I5" s="8" t="inlineStr">
+        <is>
+          <t>Cost</t>
         </is>
       </c>
       <c r="J5" s="8" t="inlineStr">
         <is>
-          <t>Cost</t>
-        </is>
-      </c>
-      <c r="K5" s="8" t="inlineStr">
-        <is>
           <t>Ext.</t>
+        </is>
+      </c>
+      <c r="K5" s="7" t="inlineStr">
+        <is>
+          <t>Stock*</t>
         </is>
       </c>
       <c r="L5" s="7" t="inlineStr">
@@ -389,7 +382,7 @@
           <t>C1, C2</t>
         </is>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D6" t="s">
@@ -408,14 +401,14 @@
         <v>6</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="J6">
-        <v>0.14299999999999999</v>
+        <f>I6*A6</f>
+        <v>0.28599999999999998</v>
       </c>
       <c r="K6">
-        <f>J6*A6</f>
-        <v>0.28599999999999998</v>
+        <v>0</v>
       </c>
       <c r="L6" t="s">
         <v>7</v>
@@ -435,7 +428,7 @@
           <t>C3, C4</t>
         </is>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
@@ -457,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="J7">
+        <f>I7*A7</f>
         <v>0</v>
       </c>
       <c r="K7">
-        <f>J7*A7</f>
         <v>0</v>
       </c>
       <c r="L7" t="s">
@@ -476,7 +469,7 @@
           <t>C5, C6, C7, C8, C9, C10, C11</t>
         </is>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D8" t="s">
@@ -501,14 +494,14 @@
         </is>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="J8">
-        <v>0.57499999999999996</v>
+        <f>I8*A8</f>
+        <v>4.0249999999999995</v>
       </c>
       <c r="K8">
-        <f>J8*A8</f>
-        <v>4.0249999999999995</v>
+        <v>0</v>
       </c>
       <c r="L8" t="s">
         <v>7</v>
@@ -528,7 +521,7 @@
           <t>CM1.1, CM1.2, CM1.3, CM2.2, CM2.3, CM3.2, CM4.1</t>
         </is>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D9" t="s">
@@ -553,14 +546,14 @@
         </is>
       </c>
       <c r="I9">
+        <v>14.02</v>
+      </c>
+      <c r="J9">
+        <f>I9*A9</f>
+        <v>98.140000000000001</v>
+      </c>
+      <c r="K9">
         <v>8</v>
-      </c>
-      <c r="J9">
-        <v>14.02</v>
-      </c>
-      <c r="K9">
-        <f>J9*A9</f>
-        <v>98.140000000000001</v>
       </c>
       <c r="L9" t="s">
         <v>10</v>
@@ -580,7 +573,7 @@
           <t>B1, B2, B3, B4, B5, B6, B7</t>
         </is>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D10" t="s">
@@ -605,17 +598,22 @@
         </is>
       </c>
       <c r="I10">
+        <v>14.720000000000001</v>
+      </c>
+      <c r="J10">
+        <f>I10*A10</f>
+        <v>103.04000000000001</v>
+      </c>
+      <c r="K10">
         <v>16</v>
-      </c>
-      <c r="J10">
-        <v>14.720000000000001</v>
-      </c>
-      <c r="K10">
-        <f>J10*A10</f>
-        <v>103.04000000000001</v>
       </c>
       <c r="L10" t="s">
         <v>10</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>RF barrel adapters (required)</t>
+        </is>
       </c>
     </row>
     <row r="11" spans="1:21" ht="13.5">
@@ -627,7 +625,7 @@
           <t>CF1.2, CF2.2, CF3.2, CF4.2, CF5.2, CF6.2, CF7.2, CF8.2</t>
         </is>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D11" t="inlineStr">
@@ -654,14 +652,14 @@
         </is>
       </c>
       <c r="I11">
+        <v>11.997999999999999</v>
+      </c>
+      <c r="J11">
+        <f>I11*A11</f>
+        <v>83.98599999999999</v>
+      </c>
+      <c r="K11">
         <v>11</v>
-      </c>
-      <c r="J11">
-        <v>11.997999999999999</v>
-      </c>
-      <c r="K11">
-        <f>J11*A11</f>
-        <v>83.98599999999999</v>
       </c>
       <c r="L11" t="s">
         <v>10</v>
@@ -681,22 +679,22 @@
           <t>J1</t>
         </is>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Hawin</t>
+          <t>TE</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>M55-6001642R</t>
+          <t>5-104196-5</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>20 Position Receptacle Connector  Through Hole, Right Angle</t>
+          <t>20 Position Receptacle Connector 0.050" (1.27mm) Through Hole, Right Angle Gold</t>
         </is>
       </c>
       <c r="G12" t="s">
@@ -708,14 +706,14 @@
         </is>
       </c>
       <c r="I12">
+        <v>6.4299999999999997</v>
+      </c>
+      <c r="J12">
+        <f>I12*A12</f>
+        <v>6.4299999999999997</v>
+      </c>
+      <c r="K12">
         <v>8</v>
-      </c>
-      <c r="J12">
-        <v>6.4299999999999997</v>
-      </c>
-      <c r="K12">
-        <f>J12*A12</f>
-        <v>6.4299999999999997</v>
       </c>
       <c r="L12" t="s">
         <v>10</v>
@@ -732,10 +730,10 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>J3</t>
-        </is>
-      </c>
-      <c r="C13" s="1" t="s">
+          <t>J2</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D13" t="inlineStr">
@@ -745,12 +743,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>M50-3501042</t>
+          <t>M55-6001642R</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>20 Position Connector Header Through Hole 0.050" (1.27mm)</t>
+          <t>16 Position Receptacle Connector 0.050" (1.27mm) Surface Mount Gold</t>
         </is>
       </c>
       <c r="G13" t="s">
@@ -758,18 +756,18 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>952-1386-ND</t>
+          <t>952-3836-1-ND</t>
         </is>
       </c>
       <c r="I13">
-        <v>3</v>
+        <v>1.96</v>
       </c>
       <c r="J13">
-        <v>1.78</v>
+        <f>I13*A13</f>
+        <v>1.96</v>
       </c>
       <c r="K13">
-        <f>J13*A13</f>
-        <v>1.78</v>
+        <v>6</v>
       </c>
       <c r="L13" t="s">
         <v>10</v>
@@ -782,237 +780,315 @@
     </row>
     <row r="14" spans="1:21" ht="13.5">
       <c r="A14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R1, R2, R3, R4</t>
-        </is>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
+          <t>PCB1</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Osh Park</t>
+        </is>
+      </c>
+      <c r="E14" t="s">
         <v>11</v>
       </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" t="s">
-        <v>13</v>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>OreSat0 1U Backplane v2.0</t>
+        </is>
       </c>
       <c r="G14" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>126.59999999999999</v>
       </c>
       <c r="J14">
-        <v>0.126</v>
+        <f>I14*A14</f>
+        <v>126.59999999999999</v>
       </c>
       <c r="K14">
-        <f>J14*A14</f>
-        <v>0.504</v>
+        <v>3</v>
       </c>
       <c r="L14" t="s">
-        <v>7</v>
-      </c>
-      <c r="M14" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>4 layer Osh Park PCB</t>
+        </is>
       </c>
     </row>
     <row r="15" spans="1:21" ht="13.5">
       <c r="A15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R5, R6, R7, R8</t>
-        </is>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>8</v>
+          <t>R1, R2, R3, R4</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G15" t="s">
         <v>5</v>
       </c>
       <c r="H15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>0.126</v>
       </c>
       <c r="J15">
-        <v>0.126</v>
+        <f>I15*A15</f>
+        <v>0.504</v>
       </c>
       <c r="K15">
-        <f>J15*A15</f>
         <v>0</v>
       </c>
       <c r="L15" t="s">
         <v>7</v>
       </c>
       <c r="M15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="13.5">
       <c r="A16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>R9, R10</t>
-        </is>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Stackpole</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>RMCF0603ZT0R00</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>0 Ohms Jumper 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
-        </is>
+          <t>R5, R6, R7, R8</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>RMCF0603ZT0R00CT-ND</t>
-        </is>
+      <c r="H16" t="s">
+        <v>15</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>0.126</v>
       </c>
       <c r="J16">
-        <v>0.10000000000000001</v>
+        <f>I16*A16</f>
+        <v>0</v>
       </c>
       <c r="K16">
-        <f>J16*A16</f>
-        <v>0.20000000000000001</v>
+        <v>0</v>
       </c>
       <c r="L16" t="s">
         <v>7</v>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>CAN jumpers</t>
-        </is>
+      <c r="M16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="13.5">
-      <c r="I17" s="0"/>
-      <c r="L17" s="0"/>
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>R9, R10</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Stackpole</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>RMCF0603ZT0R00</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>0 Ohms Jumper 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+        </is>
+      </c>
+      <c r="G17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>RMCF0603ZT0R00CT-ND</t>
+        </is>
+      </c>
+      <c r="I17">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="J17">
+        <f>I17*A17</f>
+        <v>0.20000000000000001</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>CAN jumpers (bridges CAN1 to CAN2)</t>
+        </is>
+      </c>
     </row>
     <row r="18" spans="1:21" ht="13.5">
-      <c r="I18" s="0"/>
-      <c r="J18" s="5" t="inlineStr">
+      <c r="K18" s="0"/>
+      <c r="L18" s="0"/>
+    </row>
+    <row r="19" spans="1:21" ht="13.5">
+      <c r="I19" s="4" t="inlineStr">
         <is>
           <t>Total:</t>
         </is>
       </c>
-      <c r="K18" s="5">
-        <f>SUM(K6:K16)</f>
-        <v>298.39100000000002</v>
-      </c>
-      <c r="L18" s="0"/>
-    </row>
-    <row r="20" spans="1:21" ht="13.5">
-      <c r="A20" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="13.5">
-      <c r="A22" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>0</v>
+      <c r="J19" s="4">
+        <f>SUM(J6:J17)</f>
+        <v>425.17099999999999</v>
+      </c>
+      <c r="K19" s="0"/>
+      <c r="L19" s="0"/>
+    </row>
+    <row r="20" spans="1:21" ht="13.5"/>
+    <row r="21" spans="1:21" ht="13.5">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>BOM Version Information</t>
+        </is>
       </c>
     </row>
     <row r="23" spans="1:21" ht="13.5">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>1.0r0</t>
-        </is>
-      </c>
-      <c r="B23" s="9" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Initial BOM for 1U.</t>
-        </is>
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>Rev</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="13.5">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1.1r0</t>
-        </is>
-      </c>
-      <c r="B24" s="9">
-        <v>44173</v>
+          <t>1.0r0</t>
+        </is>
+      </c>
+      <c r="B24" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Added -Z end cap connector, and debug connector.</t>
+          <t>Initial BOM for 1U.</t>
         </is>
       </c>
     </row>
     <row r="25" spans="1:21" ht="13.5">
       <c r="A25" t="inlineStr">
         <is>
+          <t>1.1r0</t>
+        </is>
+      </c>
+      <c r="B25" s="9">
+        <v>44173</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Added -Z end cap connector, and debug connector.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="13.5">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>2.0r0</t>
         </is>
       </c>
-      <c r="B25" s="9">
+      <c r="B26" s="9">
         <v>44486</v>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>v2.0 backplane specifically for OreSat0</t>
         </is>
       </c>
     </row>
-    <row r="26" spans="1:21">
-      <c r="B26" s="10"/>
-    </row>
-    <row r="27" spans="1:21">
-      <c r="B27" s="10"/>
+    <row r="27" spans="1:21" ht="13.5">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2.0r1</t>
+        </is>
+      </c>
+      <c r="B27" s="9">
+        <v>44525</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Fixed debug connector.</t>
+        </is>
+      </c>
     </row>
     <row r="28" spans="1:21">
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="1:21">
-      <c r="B29" s="10"/>
+    <row r="29" spans="1:21" ht="13.5">
+      <c r="A29" s="3" t="inlineStr">
+        <is>
+          <t>* Stock:</t>
+        </is>
+      </c>
+      <c r="B29" s="9">
+        <v>44501</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Last updated before OreSat0.1 orders</t>
+        </is>
+      </c>
     </row>
     <row r="30" spans="1:21">
       <c r="B30" s="10"/>
@@ -1050,8 +1126,8 @@
     <row r="41" spans="1:21">
       <c r="B41" s="10"/>
     </row>
-    <row r="1048566" spans="1:21">
-      <c r="L1048566" s="0"/>
+    <row r="42" spans="1:21">
+      <c r="B42" s="10"/>
     </row>
     <row r="1048567" spans="1:21">
       <c r="L1048567" s="0"/>
@@ -1081,9 +1157,6 @@
       <c r="L1048575" s="0"/>
     </row>
     <row r="1048576" spans="1:21">
-      <c r="I1048576" s="0"/>
-      <c r="J1048576" s="0"/>
-      <c r="K1048576" s="0"/>
       <c r="L1048576" s="0"/>
     </row>
   </sheetData>

</xml_diff>